<commit_message>
Adjustments to excel file
</commit_message>
<xml_diff>
--- a/data/DataAreaFile.xlsx
+++ b/data/DataAreaFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6cb6b6143dae0d7/Documents/R/browser/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{05861692-9009-4441-B2D2-265253BE0AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E22DA832-E5D1-4A5A-9C55-A3D8921D3C94}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="8_{05861692-9009-4441-B2D2-265253BE0AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E05513C5-03F9-44EB-A75F-E699A37EB566}"/>
   <bookViews>
-    <workbookView xWindow="11928" yWindow="6564" windowWidth="11112" windowHeight="5640" activeTab="1" xr2:uid="{52163122-39DA-4AC1-834B-3EB0B25A5BD9}"/>
+    <workbookView xWindow="12876" yWindow="0" windowWidth="10164" windowHeight="11844" activeTab="1" xr2:uid="{52163122-39DA-4AC1-834B-3EB0B25A5BD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Climate</t>
   </si>
@@ -157,9 +157,6 @@
     <t>XXXXXXXXXX</t>
   </si>
   <si>
-    <t>eBird Observation Dataset</t>
-  </si>
-  <si>
     <t>Intermountain Herbarium (Vascular plants &amp; algae)</t>
   </si>
   <si>
@@ -182,6 +179,15 @@
   </si>
   <si>
     <t>New_Zealand_eBird.xlsx</t>
+  </si>
+  <si>
+    <t>NZ eBird Observation Dataset</t>
+  </si>
+  <si>
+    <t>UT eBird Observation Dataset</t>
+  </si>
+  <si>
+    <t>HI eBird Observation Dataset</t>
   </si>
 </sst>
 </file>
@@ -611,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF6C410-5600-45F5-A753-74F7DE3CBA5F}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -897,10 +903,10 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <v>19.719000000000001</v>
@@ -914,10 +920,10 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16">
         <v>19.719000000000001</v>
@@ -931,10 +937,10 @@
         <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17">
         <v>41.57</v>
@@ -948,10 +954,10 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18">
         <v>41.6</v>
@@ -965,10 +971,10 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19">
         <v>-44.2</v>
@@ -982,7 +988,7 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed automatic fill in for Walter-Lieth, added Samoa data, and added files to Getting Started and Learn More pages.
</commit_message>
<xml_diff>
--- a/data/DataAreaFile.xlsx
+++ b/data/DataAreaFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6cb6b6143dae0d7/Documents/R/browser/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="8_{05861692-9009-4441-B2D2-265253BE0AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E05513C5-03F9-44EB-A75F-E699A37EB566}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="8_{05861692-9009-4441-B2D2-265253BE0AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8437CA5E-9DB9-4E51-87FA-6DF796DE9DED}"/>
   <bookViews>
-    <workbookView xWindow="12876" yWindow="0" windowWidth="10164" windowHeight="11844" activeTab="1" xr2:uid="{52163122-39DA-4AC1-834B-3EB0B25A5BD9}"/>
+    <workbookView xWindow="2412" yWindow="516" windowWidth="15156" windowHeight="11844" activeTab="1" xr2:uid="{52163122-39DA-4AC1-834B-3EB0B25A5BD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,15 +49,9 @@
     <t>Logan, UT (climate)</t>
   </si>
   <si>
-    <t>Hawaii (climate)</t>
-  </si>
-  <si>
     <t>File</t>
   </si>
   <si>
-    <t>Hilo, Hawaii Intl Airport 87</t>
-  </si>
-  <si>
     <t>Dry Bread Pond</t>
   </si>
   <si>
@@ -94,9 +88,6 @@
     <t>DataType</t>
   </si>
   <si>
-    <t>Hilo_Hawaii_climate.csv</t>
-  </si>
-  <si>
     <t>Dry_Bread_Pond_climate.xlsx</t>
   </si>
   <si>
@@ -145,39 +136,15 @@
     <t>Community</t>
   </si>
   <si>
-    <t>Hawaii (community)</t>
-  </si>
-  <si>
     <t>Logan, UT (community)</t>
   </si>
   <si>
     <t>New Zealand (community)</t>
   </si>
   <si>
-    <t>XXXXXXXXXX</t>
-  </si>
-  <si>
-    <t>Intermountain Herbarium (Vascular plants &amp; algae)</t>
-  </si>
-  <si>
-    <t>iNaturalist Research-grade Observations</t>
-  </si>
-  <si>
-    <t>Plant Dataset</t>
-  </si>
-  <si>
-    <t>Hawaii_eBird.xlsx</t>
-  </si>
-  <si>
-    <t>Hawaii_plants.xlsx</t>
-  </si>
-  <si>
     <t>Logan_eBird.xlsx</t>
   </si>
   <si>
-    <t>Logan_plants.xlsx</t>
-  </si>
-  <si>
     <t>New_Zealand_eBird.xlsx</t>
   </si>
   <si>
@@ -187,7 +154,40 @@
     <t>UT eBird Observation Dataset</t>
   </si>
   <si>
-    <t>HI eBird Observation Dataset</t>
+    <t>National Vegetation Survey</t>
+  </si>
+  <si>
+    <t>Forest Inventory and Analysis Dataset</t>
+  </si>
+  <si>
+    <t>Utah_Vegetation.xlsx</t>
+  </si>
+  <si>
+    <t>NZ_Vegetation.xlsx</t>
+  </si>
+  <si>
+    <t>FIA Data Description</t>
+  </si>
+  <si>
+    <t>Utah_Vegetation_Description.xlsx</t>
+  </si>
+  <si>
+    <t>NVS Data Description</t>
+  </si>
+  <si>
+    <t>NZ_Vegetation_Description.xlsx</t>
+  </si>
+  <si>
+    <t>Samoa (climate)</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t>Samoa_climate.xlsx</t>
+  </si>
+  <si>
+    <t>XXXXXXX</t>
   </si>
 </sst>
 </file>
@@ -540,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA4CE21-1CC9-45DC-B6B6-03F730FE1CF5}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -554,7 +554,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -565,7 +565,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -573,7 +573,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -581,31 +581,23 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -617,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF6C410-5600-45F5-A753-74F7DE3CBA5F}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -635,47 +627,59 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
         <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2">
-        <v>19.719100000000001</v>
+        <v>41.41</v>
       </c>
       <c r="E2">
-        <v>-155.053</v>
+        <v>-111.54</v>
       </c>
       <c r="F2">
-        <v>11.6</v>
+        <v>2545.1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>41.41</v>
+      </c>
+      <c r="E3">
+        <v>-111.83</v>
+      </c>
+      <c r="F3">
+        <v>1994.6</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -686,16 +690,16 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4">
-        <v>41.41</v>
+        <v>41.734999999999999</v>
       </c>
       <c r="E4">
-        <v>-111.54</v>
+        <v>-111.85639999999999</v>
       </c>
       <c r="F4">
-        <v>2545.1</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -706,56 +710,56 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5">
-        <v>41.41</v>
+        <v>41.745600000000003</v>
       </c>
       <c r="E5">
-        <v>-111.83</v>
+        <v>-111.80329999999999</v>
       </c>
       <c r="F5">
-        <v>1994.6</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D6">
-        <v>41.734999999999999</v>
+        <v>-43.365479999999998</v>
       </c>
       <c r="E6">
-        <v>-111.85639999999999</v>
+        <v>170.13427999999999</v>
       </c>
       <c r="F6">
-        <v>1364</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D7">
-        <v>41.745600000000003</v>
+        <v>-44.634659999999997</v>
       </c>
       <c r="E7">
-        <v>-111.80329999999999</v>
+        <v>170.64731</v>
       </c>
       <c r="F7">
-        <v>1460</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -766,16 +770,16 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D8">
-        <v>-43.365479999999998</v>
+        <v>-44.732999999999997</v>
       </c>
       <c r="E8">
-        <v>170.13427999999999</v>
+        <v>170.46700000000001</v>
       </c>
       <c r="F8">
-        <v>80</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -786,16 +790,16 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D9">
-        <v>-44.634659999999997</v>
+        <v>-44.001730000000002</v>
       </c>
       <c r="E9">
-        <v>170.64731</v>
+        <v>170.44318999999999</v>
       </c>
       <c r="F9">
-        <v>355</v>
+        <v>762</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -806,16 +810,16 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D10">
-        <v>-44.732999999999997</v>
+        <v>-43.735999999999997</v>
       </c>
       <c r="E10">
-        <v>170.46700000000001</v>
+        <v>170.096</v>
       </c>
       <c r="F10">
-        <v>207</v>
+        <v>730</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -826,16 +830,16 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11">
-        <v>-44.001730000000002</v>
+        <v>-43.721539999999997</v>
       </c>
       <c r="E11">
-        <v>170.44318999999999</v>
+        <v>170.06493</v>
       </c>
       <c r="F11">
-        <v>762</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -846,149 +850,125 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12">
-        <v>-43.735999999999997</v>
+        <v>-45.1</v>
       </c>
       <c r="E12">
-        <v>170.096</v>
+        <v>170.95</v>
       </c>
       <c r="F12">
-        <v>730</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D13">
-        <v>-43.721539999999997</v>
+        <v>-13.759</v>
       </c>
       <c r="E13">
-        <v>170.06493</v>
+        <v>-172.1046</v>
       </c>
       <c r="F13">
-        <v>1818</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14">
-        <v>-45.1</v>
-      </c>
-      <c r="E14">
-        <v>170.95</v>
-      </c>
-      <c r="F14">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D15">
-        <v>19.719000000000001</v>
+        <v>41.57</v>
       </c>
       <c r="E15">
-        <v>-155.05000000000001</v>
+        <v>-111.7</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
         <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16">
-        <v>19.719000000000001</v>
-      </c>
-      <c r="E16">
-        <v>-155.05000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17">
-        <v>41.57</v>
-      </c>
-      <c r="E17">
-        <v>-111.7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D18">
-        <v>41.6</v>
+        <v>-44.2</v>
       </c>
       <c r="E18">
-        <v>-111.65</v>
+        <v>170.5</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19">
-        <v>-44.2</v>
-      </c>
-      <c r="E19">
-        <v>170.5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Samoa Projection Data
</commit_message>
<xml_diff>
--- a/data/DataAreaFile.xlsx
+++ b/data/DataAreaFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6cb6b6143dae0d7/Documents/R/browser/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="8_{05861692-9009-4441-B2D2-265253BE0AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC80221A-6D44-4A0A-B436-FC2E7EE73042}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="8_{05861692-9009-4441-B2D2-265253BE0AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5FB5B31-0BE3-42E6-9984-043654D005BD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{52163122-39DA-4AC1-834B-3EB0B25A5BD9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>Climate</t>
   </si>
@@ -178,10 +178,13 @@
     <t>Samoa</t>
   </si>
   <si>
-    <t>XXXXXXX</t>
-  </si>
-  <si>
     <t>Samoa_Climate.xlsx</t>
+  </si>
+  <si>
+    <t>Samoa Projection Data</t>
+  </si>
+  <si>
+    <t>Samoa_Climate_Projection.xlsx</t>
   </si>
 </sst>
 </file>
@@ -604,7 +607,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -844,7 +847,7 @@
         <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12">
         <v>-13.759</v>
@@ -861,10 +864,19 @@
         <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="D13">
+        <v>-13.759</v>
+      </c>
+      <c r="E13">
+        <v>-172.1046</v>
+      </c>
+      <c r="F13">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:6">

</xml_diff>